<commit_message>
Adding the hypothesis testing
</commit_message>
<xml_diff>
--- a/Prueba con otros datos/songstats.xlsx
+++ b/Prueba con otros datos/songstats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/Desktop/UC3M/Curso 2/1º Cuatrimestre/Statistic/Satistics Final Project/Prueba con otros datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/Desktop/UC3M/Satistics Final Project/Prueba con otros datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0899D2CB-99D0-FE40-97AC-6CA4DDF2D5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A65C9F0-1B71-9147-B347-D38E56EAC217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="500" windowWidth="27880" windowHeight="17500" xr2:uid="{1E92F581-86EA-2D46-99A1-0B3CE0122B65}"/>
+    <workbookView xWindow="-22400" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{1E92F581-86EA-2D46-99A1-0B3CE0122B65}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="22">
   <si>
     <t>danceability</t>
   </si>
@@ -109,6 +109,12 @@
   <si>
     <t>duration_s</t>
   </si>
+  <si>
+    <t>rithmM</t>
+  </si>
+  <si>
+    <t>rithmF</t>
+  </si>
 </sst>
 </file>
 
@@ -160,21 +166,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -186,6 +188,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -202,8 +207,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{88BAD4E2-4CA4-7842-B4DF-E0AD396FDAD3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="27" unboundColumnsRight="1">
-    <queryTableFields count="13">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="29" unboundColumnsRight="3">
+    <queryTableFields count="15">
       <queryTableField id="1" name="danceability" tableColumnId="1"/>
       <queryTableField id="2" name="energy" tableColumnId="2"/>
       <queryTableField id="25" dataBound="0" tableColumnId="5"/>
@@ -217,6 +222,8 @@
       <queryTableField id="11" name="tempo" tableColumnId="11"/>
       <queryTableField id="12" name="duration_ms" tableColumnId="12"/>
       <queryTableField id="15" dataBound="0" tableColumnId="15"/>
+      <queryTableField id="27" dataBound="0" tableColumnId="8"/>
+      <queryTableField id="28" dataBound="0" tableColumnId="13"/>
     </queryTableFields>
     <queryTableDeletedFields count="6">
       <deletedField name="key"/>
@@ -231,22 +238,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F98DCAC7-C9D2-0A4E-AC7F-DE7D859511C6}" name="data" displayName="data" ref="A1:M168" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M168" xr:uid="{F98DCAC7-C9D2-0A4E-AC7F-DE7D859511C6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F98DCAC7-C9D2-0A4E-AC7F-DE7D859511C6}" name="data" displayName="data" ref="A1:O168" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:O168" xr:uid="{F98DCAC7-C9D2-0A4E-AC7F-DE7D859511C6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M168">
     <sortCondition ref="B1:B168"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{93077C1F-F2D1-E549-BAEF-E908DC199365}" uniqueName="1" name="danceability" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{B161D1B2-CB28-6B40-BC1D-03CF7C7D9710}" uniqueName="2" name="energy" queryTableFieldId="2"/>
-    <tableColumn id="5" xr3:uid="{78E9B68B-F3B1-0446-B43C-C7AD011AC1D3}" uniqueName="5" name="rithm" queryTableFieldId="25" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{78E9B68B-F3B1-0446-B43C-C7AD011AC1D3}" uniqueName="5" name="rithm" queryTableFieldId="25" dataDxfId="4">
       <calculatedColumnFormula>D2*E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BB2CA601-AB39-1A49-B81A-A3A40C33994B}" uniqueName="3" name="rithm_base" queryTableFieldId="22" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{BB2CA601-AB39-1A49-B81A-A3A40C33994B}" uniqueName="3" name="rithm_base" queryTableFieldId="22" dataDxfId="3">
       <calculatedColumnFormula>B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A8F66F67-2363-FA46-AB05-F9BC2C49CAC5}" uniqueName="4" name="rng" queryTableFieldId="24" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{35A5B1F8-C11B-5D4D-879E-57658DA1CCC2}" uniqueName="21" name="loudness" queryTableFieldId="21" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A8F66F67-2363-FA46-AB05-F9BC2C49CAC5}" uniqueName="4" name="rng" queryTableFieldId="24" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{35A5B1F8-C11B-5D4D-879E-57658DA1CCC2}" uniqueName="21" name="loudness" queryTableFieldId="21" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{CF82051B-2C61-8448-9C0B-301040AF7B5D}" uniqueName="6" name="speechiness" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{D5207915-7E24-8B4D-9701-2BD89780BD22}" uniqueName="7" name="acousticness" queryTableFieldId="7"/>
     <tableColumn id="9" xr3:uid="{F4701930-33CB-2B47-BF8E-F8155D15C3E7}" uniqueName="9" name="liveness" queryTableFieldId="9"/>
@@ -254,6 +261,8 @@
     <tableColumn id="11" xr3:uid="{3D08CAE3-C257-C047-AC18-97354A4B01FC}" uniqueName="11" name="tempo" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{10BB4036-8316-5741-98F6-412D6FBDFEFF}" uniqueName="12" name="duration_s" queryTableFieldId="12" dataDxfId="0"/>
     <tableColumn id="15" xr3:uid="{E8EF366D-E798-5B44-9D35-626BB7AEB31C}" uniqueName="15" name="GenderGroup" queryTableFieldId="15"/>
+    <tableColumn id="8" xr3:uid="{7F2A1311-6572-C640-8861-FC60285A5112}" uniqueName="8" name="rithmM" queryTableFieldId="27"/>
+    <tableColumn id="13" xr3:uid="{416AD117-39F3-934C-846F-C40AD06AA416}" uniqueName="13" name="rithmF" queryTableFieldId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -556,27 +565,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09B72C2-0037-C948-AD8B-733A23CC0ED7}">
-  <dimension ref="A1:M168"/>
+  <dimension ref="A1:O168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="157" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +619,7 @@
       <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
       <c r="L1" t="s">
@@ -616,8 +628,14 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>267</v>
       </c>
@@ -658,8 +676,14 @@
       <c r="M2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="4">
+        <v>340.60235593192584</v>
+      </c>
+      <c r="O2" s="4">
+        <v>412.13230065319232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>368</v>
       </c>
@@ -700,8 +724,14 @@
       <c r="M3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="4">
+        <v>822.45349818176942</v>
+      </c>
+      <c r="O3" s="4">
+        <v>596.72884044918737</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>334</v>
       </c>
@@ -733,7 +763,7 @@
       <c r="J4">
         <v>9.64E-2</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4">
         <v>60.170999999999999</v>
       </c>
       <c r="L4" s="4">
@@ -742,8 +772,14 @@
       <c r="M4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="4">
+        <v>372.29651812577958</v>
+      </c>
+      <c r="O4" s="4">
+        <v>666.80017071024974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>335</v>
       </c>
@@ -784,8 +820,14 @@
       <c r="M5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="4">
+        <v>741.58235777671337</v>
+      </c>
+      <c r="O5" s="4">
+        <v>162.83409376040422</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>191</v>
       </c>
@@ -826,8 +868,14 @@
       <c r="M6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="4">
+        <v>670.42268413549505</v>
+      </c>
+      <c r="O6" s="4">
+        <v>425.23061608536591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>230</v>
       </c>
@@ -868,8 +916,14 @@
       <c r="M7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="4">
+        <v>104.92794762815716</v>
+      </c>
+      <c r="O7" s="4">
+        <v>467.67837019588745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>307</v>
       </c>
@@ -910,8 +964,14 @@
       <c r="M8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="4">
+        <v>138.81219506018985</v>
+      </c>
+      <c r="O8" s="4">
+        <v>518.5933500243143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>392</v>
       </c>
@@ -952,8 +1012,14 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="4">
+        <v>162.34655088683019</v>
+      </c>
+      <c r="O9" s="4">
+        <v>368.03086228544419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>166</v>
       </c>
@@ -994,8 +1060,14 @@
       <c r="M10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="4">
+        <v>301.31502487352668</v>
+      </c>
+      <c r="O10" s="4">
+        <v>547.98021911099931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>191</v>
       </c>
@@ -1036,8 +1108,14 @@
       <c r="M11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="4">
+        <v>364.4805597129249</v>
+      </c>
+      <c r="O11" s="4">
+        <v>542.81324788474092</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>318</v>
       </c>
@@ -1078,8 +1156,14 @@
       <c r="M12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="4">
+        <v>536.19991254520994</v>
+      </c>
+      <c r="O12" s="4">
+        <v>573.46458098152459</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>213</v>
       </c>
@@ -1120,8 +1204,14 @@
       <c r="M13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="4">
+        <v>448.24136127706453</v>
+      </c>
+      <c r="O13" s="4">
+        <v>545.10657669019099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>379</v>
       </c>
@@ -1153,7 +1243,7 @@
       <c r="J14">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14">
         <v>68.231999999999999</v>
       </c>
       <c r="L14" s="4">
@@ -1162,8 +1252,14 @@
       <c r="M14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="4">
+        <v>485.86128259344224</v>
+      </c>
+      <c r="O14" s="4">
+        <v>665.8730763091362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>438</v>
       </c>
@@ -1204,8 +1300,14 @@
       <c r="M15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="4">
+        <v>612.33891202149448</v>
+      </c>
+      <c r="O15" s="4">
+        <v>712.92459826495417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>280</v>
       </c>
@@ -1217,7 +1319,7 @@
         <v>104.92794762815716</v>
       </c>
       <c r="D16">
-        <f>B16</f>
+        <f t="shared" ref="D16:D33" si="1">B16</f>
         <v>104</v>
       </c>
       <c r="E16" s="3">
@@ -1247,8 +1349,14 @@
       <c r="M16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="4">
+        <v>523.14247171524744</v>
+      </c>
+      <c r="O16" s="4">
+        <v>552.51408703559252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>205</v>
       </c>
@@ -1260,7 +1368,7 @@
         <v>138.81219506018985</v>
       </c>
       <c r="D17">
-        <f>B17</f>
+        <f t="shared" si="1"/>
         <v>129</v>
       </c>
       <c r="E17" s="3">
@@ -1290,8 +1398,14 @@
       <c r="M17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="4">
+        <v>518.18086247094868</v>
+      </c>
+      <c r="O17" s="4">
+        <v>699.05193136809737</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>463</v>
       </c>
@@ -1303,7 +1417,7 @@
         <v>162.83409376040422</v>
       </c>
       <c r="D18">
-        <f>B18</f>
+        <f t="shared" si="1"/>
         <v>155</v>
       </c>
       <c r="E18" s="3">
@@ -1333,8 +1447,14 @@
       <c r="M18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="4">
+        <v>625.21217093863083</v>
+      </c>
+      <c r="O18" s="4">
+        <v>590.253156253783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>263</v>
       </c>
@@ -1346,7 +1466,7 @@
         <v>162.34655088683019</v>
       </c>
       <c r="D19">
-        <f>B19</f>
+        <f t="shared" si="1"/>
         <v>202</v>
       </c>
       <c r="E19" s="3">
@@ -1376,8 +1496,14 @@
       <c r="M19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="4">
+        <v>511.63816519666761</v>
+      </c>
+      <c r="O19" s="4">
+        <v>581.26134388493119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>657</v>
       </c>
@@ -1389,7 +1515,7 @@
         <v>301.31502487352668</v>
       </c>
       <c r="D20">
-        <f>B20</f>
+        <f t="shared" si="1"/>
         <v>333</v>
       </c>
       <c r="E20" s="3">
@@ -1419,8 +1545,14 @@
       <c r="M20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="4">
+        <v>495.57907636809784</v>
+      </c>
+      <c r="O20" s="4">
+        <v>752.42302120878628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>499</v>
       </c>
@@ -1432,7 +1564,7 @@
         <v>401.60469555471656</v>
       </c>
       <c r="D21">
-        <f>B21</f>
+        <f t="shared" si="1"/>
         <v>351</v>
       </c>
       <c r="E21" s="3">
@@ -1462,8 +1594,14 @@
       <c r="M21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="4">
+        <v>709.17499850027798</v>
+      </c>
+      <c r="O21" s="4">
+        <v>766.42657077154172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>235</v>
       </c>
@@ -1475,7 +1613,7 @@
         <v>301.80329894143085</v>
       </c>
       <c r="D22">
-        <f>B22</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="E22" s="3">
@@ -1505,8 +1643,14 @@
       <c r="M22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="4">
+        <v>496.96075997298516</v>
+      </c>
+      <c r="O22" s="4">
+        <v>830.51442917780719</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>592</v>
       </c>
@@ -1518,7 +1662,7 @@
         <v>340.17179594380616</v>
       </c>
       <c r="D23">
-        <f>B23</f>
+        <f t="shared" si="1"/>
         <v>371</v>
       </c>
       <c r="E23" s="3">
@@ -1548,8 +1692,14 @@
       <c r="M23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="4">
+        <v>544.67019373862149</v>
+      </c>
+      <c r="O23" s="4">
+        <v>879.6346678751031</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>656</v>
       </c>
@@ -1561,7 +1711,7 @@
         <v>346.71886899834459</v>
       </c>
       <c r="D24">
-        <f>B24</f>
+        <f t="shared" si="1"/>
         <v>381</v>
       </c>
       <c r="E24" s="3">
@@ -1591,8 +1741,14 @@
       <c r="M24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="4">
+        <v>530.46661417270468</v>
+      </c>
+      <c r="O24" s="4">
+        <v>717.68088000683042</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>583</v>
       </c>
@@ -1604,7 +1760,7 @@
         <v>423.56224987989782</v>
       </c>
       <c r="D25">
-        <f>B25</f>
+        <f t="shared" si="1"/>
         <v>381</v>
       </c>
       <c r="E25" s="3">
@@ -1634,8 +1790,14 @@
       <c r="M25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="4">
+        <v>560.31091322498298</v>
+      </c>
+      <c r="O25" s="4">
+        <v>999.00000000000011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>740</v>
       </c>
@@ -1647,7 +1809,7 @@
         <v>364.4805597129249</v>
       </c>
       <c r="D26">
-        <f>B26</f>
+        <f t="shared" si="1"/>
         <v>403</v>
       </c>
       <c r="E26" s="3">
@@ -1677,8 +1839,14 @@
       <c r="M26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="4">
+        <v>680.84064775313959</v>
+      </c>
+      <c r="O26" s="4">
+        <v>900.27800187087564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>734</v>
       </c>
@@ -1690,7 +1858,7 @@
         <v>509.09053845350883</v>
       </c>
       <c r="D27">
-        <f>B27</f>
+        <f t="shared" si="1"/>
         <v>425</v>
       </c>
       <c r="E27" s="3">
@@ -1720,8 +1888,14 @@
       <c r="M27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="4">
+        <v>694.05516982669224</v>
+      </c>
+      <c r="O27" s="4">
+        <v>827.15640105056457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>816</v>
       </c>
@@ -1733,7 +1907,7 @@
         <v>425.23061608536591</v>
       </c>
       <c r="D28">
-        <f>B28</f>
+        <f t="shared" si="1"/>
         <v>433</v>
       </c>
       <c r="E28" s="3">
@@ -1763,8 +1937,14 @@
       <c r="M28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" s="4">
+        <v>765.04883774200528</v>
+      </c>
+      <c r="O28" s="4">
+        <v>983.43431522243338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>447</v>
       </c>
@@ -1776,7 +1956,7 @@
         <v>467.67837019588745</v>
       </c>
       <c r="D29">
-        <f>B29</f>
+        <f t="shared" si="1"/>
         <v>449</v>
       </c>
       <c r="E29" s="3">
@@ -1806,8 +1986,14 @@
       <c r="M29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" s="4">
+        <v>645.49173318384169</v>
+      </c>
+      <c r="O29" s="4">
+        <v>1011.6658688265728</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>757</v>
       </c>
@@ -1819,7 +2005,7 @@
         <v>443.00530381223939</v>
       </c>
       <c r="D30">
-        <f>B30</f>
+        <f t="shared" si="1"/>
         <v>451</v>
       </c>
       <c r="E30" s="3">
@@ -1849,8 +2035,14 @@
       <c r="M30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" s="4">
+        <v>564.60727022777962</v>
+      </c>
+      <c r="O30" s="4">
+        <v>855.50207451273684</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>745</v>
       </c>
@@ -1862,7 +2054,7 @@
         <v>444.4829867278811</v>
       </c>
       <c r="D31">
-        <f>B31</f>
+        <f t="shared" si="1"/>
         <v>456</v>
       </c>
       <c r="E31" s="3">
@@ -1892,8 +2084,14 @@
       <c r="M31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" s="4">
+        <v>640.43662557221137</v>
+      </c>
+      <c r="O31" s="4">
+        <v>764.05325196617218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>456</v>
       </c>
@@ -1905,7 +2103,7 @@
         <v>522.86653153418933</v>
       </c>
       <c r="D32">
-        <f>B32</f>
+        <f t="shared" si="1"/>
         <v>456</v>
       </c>
       <c r="E32" s="3">
@@ -1935,8 +2133,14 @@
       <c r="M32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" s="4">
+        <v>661.1139232414971</v>
+      </c>
+      <c r="O32" s="4">
+        <v>784.11830266730203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>867</v>
       </c>
@@ -1948,7 +2152,7 @@
         <v>518.5933500243143</v>
       </c>
       <c r="D33">
-        <f>B33</f>
+        <f t="shared" si="1"/>
         <v>457</v>
       </c>
       <c r="E33" s="3">
@@ -1978,8 +2182,14 @@
       <c r="M33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="4">
+        <v>728.47457546257681</v>
+      </c>
+      <c r="O33" s="4">
+        <v>777.82723633726528</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>668</v>
       </c>
@@ -1987,11 +2197,11 @@
         <v>459</v>
       </c>
       <c r="C34" s="4">
-        <f t="shared" ref="C34:C65" si="1">D34*E34</f>
+        <f t="shared" ref="C34:C65" si="2">D34*E34</f>
         <v>368.03086228544419</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D65" si="2">B34</f>
+        <f t="shared" ref="D34:D65" si="3">B34</f>
         <v>459</v>
       </c>
       <c r="E34" s="3">
@@ -2021,8 +2231,14 @@
       <c r="M34" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="4">
+        <v>641.88936008811129</v>
+      </c>
+      <c r="O34" s="4">
+        <v>975.47763584211941</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>752</v>
       </c>
@@ -2030,11 +2246,11 @@
         <v>468</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>547.98021911099931</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>468</v>
       </c>
       <c r="E35" s="3">
@@ -2064,8 +2280,14 @@
       <c r="M35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="4">
+        <v>699.11203241318594</v>
+      </c>
+      <c r="O35" s="4">
+        <v>843.62034307532576</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>797</v>
       </c>
@@ -2073,11 +2295,11 @@
         <v>468</v>
       </c>
       <c r="C36" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>375.16597899372039</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>468</v>
       </c>
       <c r="E36" s="3">
@@ -2107,8 +2329,14 @@
       <c r="M36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="4">
+        <v>816.88193392604967</v>
+      </c>
+      <c r="O36" s="4">
+        <v>1138.0076919374487</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>608</v>
       </c>
@@ -2116,11 +2344,11 @@
         <v>471</v>
       </c>
       <c r="C37" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>380.76802263943353</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>471</v>
       </c>
       <c r="E37" s="3">
@@ -2150,8 +2378,14 @@
       <c r="M37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="4">
+        <v>883.91032811598097</v>
+      </c>
+      <c r="O37" s="4">
+        <v>846.18691932122363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>875</v>
       </c>
@@ -2159,11 +2393,11 @@
         <v>474</v>
       </c>
       <c r="C38" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>420.3096445142429</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>474</v>
       </c>
       <c r="E38" s="3">
@@ -2193,8 +2427,14 @@
       <c r="M38" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" s="4">
+        <v>821.98171610899249</v>
+      </c>
+      <c r="O38" s="4">
+        <v>775.51445688586773</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>754</v>
       </c>
@@ -2202,11 +2442,11 @@
         <v>475</v>
       </c>
       <c r="C39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>542.81324788474092</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>475</v>
       </c>
       <c r="E39" s="3">
@@ -2236,8 +2476,11 @@
       <c r="M39" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" s="4">
+        <v>798.10154221300434</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>895</v>
       </c>
@@ -2245,11 +2488,11 @@
         <v>479</v>
       </c>
       <c r="C40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>536.19991254520994</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>479</v>
       </c>
       <c r="E40" s="3">
@@ -2279,8 +2522,11 @@
       <c r="M40" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" s="4">
+        <v>682.36461353777611</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>539</v>
       </c>
@@ -2288,11 +2534,11 @@
         <v>487</v>
       </c>
       <c r="C41" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>573.46458098152459</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>487</v>
       </c>
       <c r="E41" s="3">
@@ -2322,8 +2568,11 @@
       <c r="M41" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" s="4">
+        <v>758.51750567731438</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>795</v>
       </c>
@@ -2331,11 +2580,11 @@
         <v>492</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>448.24136127706453</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>492</v>
       </c>
       <c r="E42" s="3">
@@ -2365,8 +2614,11 @@
       <c r="M42" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" s="4">
+        <v>676.69812683168027</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>791</v>
       </c>
@@ -2374,11 +2626,11 @@
         <v>500</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>537.75712851571143</v>
       </c>
       <c r="D43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="E43" s="3">
@@ -2408,8 +2660,11 @@
       <c r="M43" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" s="4">
+        <v>914.86348950739819</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>609</v>
       </c>
@@ -2417,11 +2672,11 @@
         <v>517</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>545.10657669019099</v>
       </c>
       <c r="D44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>517</v>
       </c>
       <c r="E44" s="3">
@@ -2451,8 +2706,11 @@
       <c r="M44" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" s="4">
+        <v>776.12654818568558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>729</v>
       </c>
@@ -2460,11 +2718,11 @@
         <v>533</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>485.86128259344224</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>533</v>
       </c>
       <c r="E45" s="3">
@@ -2494,8 +2752,11 @@
       <c r="M45" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" s="4">
+        <v>774.47903600882853</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>616</v>
       </c>
@@ -2503,11 +2764,11 @@
         <v>534</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>612.33891202149448</v>
       </c>
       <c r="D46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>534</v>
       </c>
       <c r="E46" s="3">
@@ -2537,8 +2798,11 @@
       <c r="M46" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46" s="4">
+        <v>727.23352078063658</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>600</v>
       </c>
@@ -2546,11 +2810,11 @@
         <v>535</v>
       </c>
       <c r="C47" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>514.57579566700758</v>
       </c>
       <c r="D47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>535</v>
       </c>
       <c r="E47" s="3">
@@ -2580,8 +2844,11 @@
       <c r="M47" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" s="4">
+        <v>770.70090825830027</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>792</v>
       </c>
@@ -2589,11 +2856,11 @@
         <v>536</v>
       </c>
       <c r="C48" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>439.92097120359978</v>
       </c>
       <c r="D48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>536</v>
       </c>
       <c r="E48" s="3">
@@ -2623,8 +2890,11 @@
       <c r="M48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" s="4">
+        <v>778.42911780216275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>802</v>
       </c>
@@ -2632,11 +2902,11 @@
         <v>549</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>523.14247171524744</v>
       </c>
       <c r="D49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>549</v>
       </c>
       <c r="E49" s="3">
@@ -2666,8 +2936,11 @@
       <c r="M49" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49" s="4">
+        <v>859.73600982930407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>915</v>
       </c>
@@ -2675,11 +2948,11 @@
         <v>551</v>
       </c>
       <c r="C50" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>518.18086247094868</v>
       </c>
       <c r="D50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>551</v>
       </c>
       <c r="E50" s="3">
@@ -2709,8 +2982,11 @@
       <c r="M50" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50" s="4">
+        <v>1161.1614839406413</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>780</v>
       </c>
@@ -2718,11 +2994,11 @@
         <v>551</v>
       </c>
       <c r="C51" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>630.23048711526667</v>
       </c>
       <c r="D51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>551</v>
       </c>
       <c r="E51" s="3">
@@ -2752,8 +3028,11 @@
       <c r="M51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51" s="4">
+        <v>639.51338361095475</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>832</v>
       </c>
@@ -2761,11 +3040,11 @@
         <v>553</v>
       </c>
       <c r="C52" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>475.26993391255007</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>553</v>
       </c>
       <c r="E52" s="3">
@@ -2796,7 +3075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>826</v>
       </c>
@@ -2804,11 +3083,11 @@
         <v>556</v>
       </c>
       <c r="C53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>560.04027709115496</v>
       </c>
       <c r="D53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>556</v>
       </c>
       <c r="E53" s="3">
@@ -2839,7 +3118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>883</v>
       </c>
@@ -2847,11 +3126,11 @@
         <v>558</v>
       </c>
       <c r="C54" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>625.21217093863083</v>
       </c>
       <c r="D54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>558</v>
       </c>
       <c r="E54" s="3">
@@ -2882,7 +3161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>798</v>
       </c>
@@ -2890,11 +3169,11 @@
         <v>564</v>
       </c>
       <c r="C55" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>554.37924936081561</v>
       </c>
       <c r="D55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>564</v>
       </c>
       <c r="E55" s="3">
@@ -2925,7 +3204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>870</v>
       </c>
@@ -2933,11 +3212,11 @@
         <v>565</v>
       </c>
       <c r="C56" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>585.84593130543283</v>
       </c>
       <c r="D56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>565</v>
       </c>
       <c r="E56" s="3">
@@ -2968,7 +3247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>688</v>
       </c>
@@ -2976,11 +3255,11 @@
         <v>569</v>
       </c>
       <c r="C57" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>665.8730763091362</v>
       </c>
       <c r="D57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>569</v>
       </c>
       <c r="E57" s="3">
@@ -3011,7 +3290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>787</v>
       </c>
@@ -3019,11 +3298,11 @@
         <v>572</v>
       </c>
       <c r="C58" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>477.41399212257102</v>
       </c>
       <c r="D58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>572</v>
       </c>
       <c r="E58" s="3">
@@ -3054,7 +3333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>620</v>
       </c>
@@ -3062,11 +3341,11 @@
         <v>573</v>
       </c>
       <c r="C59" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>511.63816519666761</v>
       </c>
       <c r="D59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>573</v>
       </c>
       <c r="E59" s="3">
@@ -3097,7 +3376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>809</v>
       </c>
@@ -3105,11 +3384,11 @@
         <v>574</v>
       </c>
       <c r="C60" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>522.70208512027227</v>
       </c>
       <c r="D60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>574</v>
       </c>
       <c r="E60" s="3">
@@ -3140,7 +3419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>912</v>
       </c>
@@ -3148,11 +3427,11 @@
         <v>577</v>
       </c>
       <c r="C61" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>559.68055076369683</v>
       </c>
       <c r="D61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>577</v>
       </c>
       <c r="E61" s="3">
@@ -3183,7 +3462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>909</v>
       </c>
@@ -3191,11 +3470,11 @@
         <v>582</v>
       </c>
       <c r="C62" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>607.89945758440069</v>
       </c>
       <c r="D62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>582</v>
       </c>
       <c r="E62" s="3">
@@ -3226,7 +3505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>671</v>
       </c>
@@ -3234,11 +3513,11 @@
         <v>584</v>
       </c>
       <c r="C63" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>522.95538008159701</v>
       </c>
       <c r="D63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>584</v>
       </c>
       <c r="E63" s="3">
@@ -3269,7 +3548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>533</v>
       </c>
@@ -3277,11 +3556,11 @@
         <v>593</v>
       </c>
       <c r="C64" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>495.57907636809784</v>
       </c>
       <c r="D64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>593</v>
       </c>
       <c r="E64" s="3">
@@ -3320,11 +3599,11 @@
         <v>600</v>
       </c>
       <c r="C65" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>674.52853022216038</v>
       </c>
       <c r="D65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
       <c r="E65" s="3">
@@ -3363,11 +3642,11 @@
         <v>602</v>
       </c>
       <c r="C66" s="4">
-        <f t="shared" ref="C66:C97" si="3">D66*E66</f>
+        <f t="shared" ref="C66:C97" si="4">D66*E66</f>
         <v>709.17499850027798</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D97" si="4">B66</f>
+        <f t="shared" ref="D66:D97" si="5">B66</f>
         <v>602</v>
       </c>
       <c r="E66" s="3">
@@ -3406,11 +3685,11 @@
         <v>610</v>
       </c>
       <c r="C67" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>712.92459826495417</v>
       </c>
       <c r="D67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>610</v>
       </c>
       <c r="E67" s="3">
@@ -3449,11 +3728,11 @@
         <v>610</v>
       </c>
       <c r="C68" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>496.96075997298516</v>
       </c>
       <c r="D68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>610</v>
       </c>
       <c r="E68" s="3">
@@ -3492,11 +3771,11 @@
         <v>616</v>
       </c>
       <c r="C69" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>635.50298391245644</v>
       </c>
       <c r="D69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>616</v>
       </c>
       <c r="E69" s="3">
@@ -3535,11 +3814,11 @@
         <v>616</v>
       </c>
       <c r="C70" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>697.58168047067454</v>
       </c>
       <c r="D70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>616</v>
       </c>
       <c r="E70" s="3">
@@ -3578,11 +3857,11 @@
         <v>622</v>
       </c>
       <c r="C71" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>545.71826154255223</v>
       </c>
       <c r="D71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>622</v>
       </c>
       <c r="E71" s="3">
@@ -3621,11 +3900,11 @@
         <v>624</v>
       </c>
       <c r="C72" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>552.51408703559252</v>
       </c>
       <c r="D72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>624</v>
       </c>
       <c r="E72" s="3">
@@ -3664,11 +3943,11 @@
         <v>627</v>
       </c>
       <c r="C73" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>533.84528249231982</v>
       </c>
       <c r="D73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>627</v>
       </c>
       <c r="E73" s="3">
@@ -3707,11 +3986,11 @@
         <v>629</v>
       </c>
       <c r="C74" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>544.67019373862149</v>
       </c>
       <c r="D74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>629</v>
       </c>
       <c r="E74" s="3">
@@ -3750,11 +4029,11 @@
         <v>629</v>
       </c>
       <c r="C75" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>530.46661417270468</v>
       </c>
       <c r="D75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>629</v>
       </c>
       <c r="E75" s="3">
@@ -3793,11 +4072,11 @@
         <v>632</v>
       </c>
       <c r="C76" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>529.06757033138206</v>
       </c>
       <c r="D76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>632</v>
       </c>
       <c r="E76" s="3">
@@ -3836,11 +4115,11 @@
         <v>639</v>
       </c>
       <c r="C77" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>646.73544963713937</v>
       </c>
       <c r="D77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>639</v>
       </c>
       <c r="E77" s="3">
@@ -3879,11 +4158,11 @@
         <v>640</v>
       </c>
       <c r="C78" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>560.31091322498298</v>
       </c>
       <c r="D78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>640</v>
       </c>
       <c r="E78" s="3">
@@ -3922,11 +4201,11 @@
         <v>646</v>
       </c>
       <c r="C79" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>660.39294712924948</v>
       </c>
       <c r="D79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>646</v>
       </c>
       <c r="E79" s="3">
@@ -3965,11 +4244,11 @@
         <v>648</v>
       </c>
       <c r="C80" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>689.24514479422191</v>
       </c>
       <c r="D80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>648</v>
       </c>
       <c r="E80" s="3">
@@ -4008,11 +4287,11 @@
         <v>653</v>
       </c>
       <c r="C81" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>680.84064775313959</v>
       </c>
       <c r="D81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>653</v>
       </c>
       <c r="E81" s="3">
@@ -4051,11 +4330,11 @@
         <v>653</v>
       </c>
       <c r="C82" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>694.05516982669224</v>
       </c>
       <c r="D82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>653</v>
       </c>
       <c r="E82" s="3">
@@ -4094,11 +4373,11 @@
         <v>654</v>
       </c>
       <c r="C83" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>637.70638024763355</v>
       </c>
       <c r="D83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>654</v>
       </c>
       <c r="E83" s="3">
@@ -4137,11 +4416,11 @@
         <v>656</v>
       </c>
       <c r="C84" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>762.36754911744003</v>
       </c>
       <c r="D84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>656</v>
       </c>
       <c r="E84" s="3">
@@ -4180,11 +4459,11 @@
         <v>659</v>
       </c>
       <c r="C85" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>637.22899918646124</v>
       </c>
       <c r="D85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>659</v>
       </c>
       <c r="E85" s="3">
@@ -4223,11 +4502,11 @@
         <v>659</v>
       </c>
       <c r="C86" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>689.20250611023096</v>
       </c>
       <c r="D86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>659</v>
       </c>
       <c r="E86" s="3">
@@ -4266,11 +4545,11 @@
         <v>663</v>
       </c>
       <c r="C87" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>606.85767000129442</v>
       </c>
       <c r="D87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>663</v>
       </c>
       <c r="E87" s="3">
@@ -4309,11 +4588,11 @@
         <v>667</v>
       </c>
       <c r="C88" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>765.04883774200528</v>
       </c>
       <c r="D88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>667</v>
       </c>
       <c r="E88" s="3">
@@ -4352,11 +4631,11 @@
         <v>668</v>
       </c>
       <c r="C89" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>759.80587387744708</v>
       </c>
       <c r="D89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>668</v>
       </c>
       <c r="E89" s="3">
@@ -4395,11 +4674,11 @@
         <v>670</v>
       </c>
       <c r="C90" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>543.02220073457875</v>
       </c>
       <c r="D90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>670</v>
       </c>
       <c r="E90" s="3">
@@ -4438,11 +4717,11 @@
         <v>672</v>
       </c>
       <c r="C91" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>645.49173318384169</v>
       </c>
       <c r="D91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>672</v>
       </c>
       <c r="E91" s="3">
@@ -4481,11 +4760,11 @@
         <v>673</v>
       </c>
       <c r="C92" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>699.05193136809737</v>
       </c>
       <c r="D92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>673</v>
       </c>
       <c r="E92" s="3">
@@ -4524,11 +4803,11 @@
         <v>673</v>
       </c>
       <c r="C93" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>590.253156253783</v>
       </c>
       <c r="D93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>673</v>
       </c>
       <c r="E93" s="3">
@@ -4567,11 +4846,11 @@
         <v>686</v>
       </c>
       <c r="C94" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>564.60727022777962</v>
       </c>
       <c r="D94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>686</v>
       </c>
       <c r="E94" s="3">
@@ -4610,11 +4889,11 @@
         <v>698</v>
       </c>
       <c r="C95" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>581.26134388493119</v>
       </c>
       <c r="D95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>698</v>
       </c>
       <c r="E95" s="3">
@@ -4653,11 +4932,11 @@
         <v>700</v>
       </c>
       <c r="C96" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>592.781473043191</v>
       </c>
       <c r="D96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>700</v>
       </c>
       <c r="E96" s="3">
@@ -4696,11 +4975,11 @@
         <v>703</v>
       </c>
       <c r="C97" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>640.43662557221137</v>
       </c>
       <c r="D97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>703</v>
       </c>
       <c r="E97" s="3">
@@ -4721,7 +5000,7 @@
       <c r="J97">
         <v>0.58599999999999997</v>
       </c>
-      <c r="K97" s="5">
+      <c r="K97">
         <v>137.04300000000001</v>
       </c>
       <c r="L97" s="4">
@@ -4739,11 +5018,11 @@
         <v>703</v>
       </c>
       <c r="C98" s="4">
-        <f t="shared" ref="C98:C129" si="5">D98*E98</f>
+        <f t="shared" ref="C98:C129" si="6">D98*E98</f>
         <v>573.44375406064819</v>
       </c>
       <c r="D98">
-        <f t="shared" ref="D98:D129" si="6">B98</f>
+        <f t="shared" ref="D98:D129" si="7">B98</f>
         <v>703</v>
       </c>
       <c r="E98" s="3">
@@ -4764,7 +5043,7 @@
       <c r="J98">
         <v>0.51900000000000002</v>
       </c>
-      <c r="K98" s="5">
+      <c r="K98">
         <v>151.32900000000001</v>
       </c>
       <c r="L98" s="4">
@@ -4782,11 +5061,11 @@
         <v>707</v>
       </c>
       <c r="C99" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>730.74598493617452</v>
       </c>
       <c r="D99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>707</v>
       </c>
       <c r="E99" s="3">
@@ -4807,7 +5086,7 @@
       <c r="J99">
         <v>0.68200000000000005</v>
       </c>
-      <c r="K99" s="5">
+      <c r="K99">
         <v>146.154</v>
       </c>
       <c r="L99" s="4">
@@ -4825,11 +5104,11 @@
         <v>708</v>
       </c>
       <c r="C100" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>706.37667579322999</v>
       </c>
       <c r="D100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>708</v>
       </c>
       <c r="E100" s="3">
@@ -4850,7 +5129,7 @@
       <c r="J100">
         <v>0.72299999999999998</v>
       </c>
-      <c r="K100" s="5">
+      <c r="K100">
         <v>139.96100000000001</v>
       </c>
       <c r="L100" s="4">
@@ -4868,11 +5147,11 @@
         <v>715</v>
       </c>
       <c r="C101" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>820.06584501749364</v>
       </c>
       <c r="D101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>715</v>
       </c>
       <c r="E101" s="3">
@@ -4893,7 +5172,7 @@
       <c r="J101">
         <v>0.76700000000000002</v>
       </c>
-      <c r="K101" s="5">
+      <c r="K101">
         <v>140.06100000000001</v>
       </c>
       <c r="L101" s="4">
@@ -4911,11 +5190,11 @@
         <v>719</v>
       </c>
       <c r="C102" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>752.42302120878628</v>
       </c>
       <c r="D102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>719</v>
       </c>
       <c r="E102" s="3">
@@ -4936,7 +5215,7 @@
       <c r="J102">
         <v>0.42899999999999999</v>
       </c>
-      <c r="K102" s="5">
+      <c r="K102">
         <v>143.971</v>
       </c>
       <c r="L102" s="4">
@@ -4954,11 +5233,11 @@
         <v>719</v>
       </c>
       <c r="C103" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>661.1139232414971</v>
       </c>
       <c r="D103">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>719</v>
       </c>
       <c r="E103" s="3">
@@ -4979,7 +5258,7 @@
       <c r="J103">
         <v>0.81499999999999995</v>
       </c>
-      <c r="K103" s="5">
+      <c r="K103">
         <v>143.97499999999999</v>
       </c>
       <c r="L103" s="4">
@@ -4997,11 +5276,11 @@
         <v>720</v>
       </c>
       <c r="C104" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>728.47457546257681</v>
       </c>
       <c r="D104">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>720</v>
       </c>
       <c r="E104" s="3">
@@ -5022,7 +5301,7 @@
       <c r="J104">
         <v>0.76100000000000001</v>
       </c>
-      <c r="K104" s="5">
+      <c r="K104">
         <v>140.041</v>
       </c>
       <c r="L104" s="4">
@@ -5040,11 +5319,11 @@
         <v>729</v>
       </c>
       <c r="C105" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>766.42657077154172</v>
       </c>
       <c r="D105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>729</v>
       </c>
       <c r="E105" s="3">
@@ -5065,7 +5344,7 @@
       <c r="J105">
         <v>0.41299999999999998</v>
       </c>
-      <c r="K105" s="5">
+      <c r="K105">
         <v>110.547</v>
       </c>
       <c r="L105" s="4">
@@ -5083,11 +5362,11 @@
         <v>736</v>
       </c>
       <c r="C106" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>641.88936008811129</v>
       </c>
       <c r="D106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>736</v>
       </c>
       <c r="E106" s="3">
@@ -5108,7 +5387,7 @@
       <c r="J106">
         <v>0.58199999999999996</v>
       </c>
-      <c r="K106" s="5">
+      <c r="K106">
         <v>89.86</v>
       </c>
       <c r="L106" s="4">
@@ -5126,11 +5405,11 @@
         <v>743</v>
       </c>
       <c r="C107" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>699.11203241318594</v>
       </c>
       <c r="D107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>743</v>
       </c>
       <c r="E107" s="3">
@@ -5151,7 +5430,7 @@
       <c r="J107">
         <v>0.191</v>
       </c>
-      <c r="K107" s="5">
+      <c r="K107">
         <v>168.84899999999999</v>
       </c>
       <c r="L107" s="4">
@@ -5169,11 +5448,11 @@
         <v>746</v>
       </c>
       <c r="C108" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>830.51442917780719</v>
       </c>
       <c r="D108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>746</v>
       </c>
       <c r="E108" s="3">
@@ -5194,7 +5473,7 @@
       <c r="J108">
         <v>0.96499999999999997</v>
       </c>
-      <c r="K108" s="5">
+      <c r="K108">
         <v>128.553</v>
       </c>
       <c r="L108" s="4">
@@ -5212,11 +5491,11 @@
         <v>748</v>
       </c>
       <c r="C109" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>816.88193392604967</v>
       </c>
       <c r="D109">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>748</v>
       </c>
       <c r="E109" s="3">
@@ -5237,7 +5516,7 @@
       <c r="J109">
         <v>0.38100000000000001</v>
       </c>
-      <c r="K109" s="5">
+      <c r="K109">
         <v>121.063</v>
       </c>
       <c r="L109" s="4">
@@ -5255,11 +5534,11 @@
         <v>748</v>
       </c>
       <c r="C110" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>879.6346678751031</v>
       </c>
       <c r="D110">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>748</v>
       </c>
       <c r="E110" s="3">
@@ -5280,7 +5559,7 @@
       <c r="J110">
         <v>0.57999999999999996</v>
       </c>
-      <c r="K110" s="5">
+      <c r="K110">
         <v>129.43299999999999</v>
       </c>
       <c r="L110" s="4">
@@ -5298,11 +5577,11 @@
         <v>751</v>
       </c>
       <c r="C111" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>883.91032811598097</v>
       </c>
       <c r="D111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>751</v>
       </c>
       <c r="E111" s="3">
@@ -5323,7 +5602,7 @@
       <c r="J111">
         <v>0.86299999999999999</v>
       </c>
-      <c r="K111" s="5">
+      <c r="K111">
         <v>100.437</v>
       </c>
       <c r="L111" s="4">
@@ -5341,11 +5620,11 @@
         <v>758</v>
       </c>
       <c r="C112" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>821.98171610899249</v>
       </c>
       <c r="D112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>758</v>
       </c>
       <c r="E112" s="3">
@@ -5366,7 +5645,7 @@
       <c r="J112">
         <v>0.53800000000000003</v>
       </c>
-      <c r="K112" s="5">
+      <c r="K112">
         <v>131.001</v>
       </c>
       <c r="L112" s="4">
@@ -5384,11 +5663,11 @@
         <v>760</v>
       </c>
       <c r="C113" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>717.68088000683042</v>
       </c>
       <c r="D113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>760</v>
       </c>
       <c r="E113" s="3">
@@ -5409,7 +5688,7 @@
       <c r="J113">
         <v>0.81299999999999994</v>
       </c>
-      <c r="K113" s="5">
+      <c r="K113">
         <v>99.974000000000004</v>
       </c>
       <c r="L113" s="4">
@@ -5427,11 +5706,11 @@
         <v>772</v>
       </c>
       <c r="C114" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>798.10154221300434</v>
       </c>
       <c r="D114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>772</v>
       </c>
       <c r="E114" s="3">
@@ -5452,7 +5731,7 @@
       <c r="J114">
         <v>0.56100000000000005</v>
       </c>
-      <c r="K114" s="5">
+      <c r="K114">
         <v>139.97999999999999</v>
       </c>
       <c r="L114" s="4">
@@ -5470,11 +5749,11 @@
         <v>900</v>
       </c>
       <c r="C115" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>999.00000000000011</v>
       </c>
       <c r="D115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>900</v>
       </c>
       <c r="E115" s="3">
@@ -5495,7 +5774,7 @@
       <c r="J115">
         <v>0.32800000000000001</v>
       </c>
-      <c r="K115" s="5">
+      <c r="K115">
         <v>139.959</v>
       </c>
       <c r="L115" s="4">
@@ -5513,11 +5792,11 @@
         <v>797</v>
       </c>
       <c r="C116" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>772.25308014351174</v>
       </c>
       <c r="D116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>797</v>
       </c>
       <c r="E116" s="3">
@@ -5538,7 +5817,7 @@
       <c r="J116">
         <v>0.65400000000000003</v>
       </c>
-      <c r="K116" s="5">
+      <c r="K116">
         <v>110.88200000000001</v>
       </c>
       <c r="L116" s="4">
@@ -5556,11 +5835,11 @@
         <v>804</v>
       </c>
       <c r="C117" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>704.0071419712126</v>
       </c>
       <c r="D117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>804</v>
       </c>
       <c r="E117" s="3">
@@ -5599,11 +5878,11 @@
         <v>805</v>
       </c>
       <c r="C118" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>900.27800187087564</v>
       </c>
       <c r="D118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>805</v>
       </c>
       <c r="E118" s="3">
@@ -5642,11 +5921,11 @@
         <v>809</v>
       </c>
       <c r="C119" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>682.36461353777611</v>
       </c>
       <c r="D119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>809</v>
       </c>
       <c r="E119" s="3">
@@ -5685,11 +5964,11 @@
         <v>811</v>
       </c>
       <c r="C120" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>820.94081437447733</v>
       </c>
       <c r="D120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>811</v>
       </c>
       <c r="E120" s="3">
@@ -5728,11 +6007,11 @@
         <v>811</v>
       </c>
       <c r="C121" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>827.15640105056457</v>
       </c>
       <c r="D121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>811</v>
       </c>
       <c r="E121" s="3">
@@ -5771,11 +6050,11 @@
         <v>812</v>
       </c>
       <c r="C122" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>758.51750567731438</v>
       </c>
       <c r="D122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>812</v>
       </c>
       <c r="E122" s="3">
@@ -5814,11 +6093,11 @@
         <v>813</v>
       </c>
       <c r="C123" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>734.23266863450328</v>
       </c>
       <c r="D123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>813</v>
       </c>
       <c r="E123" s="3">
@@ -5857,11 +6136,11 @@
         <v>813</v>
       </c>
       <c r="C124" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>805.18775244409778</v>
       </c>
       <c r="D124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>813</v>
       </c>
       <c r="E124" s="3">
@@ -5900,11 +6179,11 @@
         <v>828</v>
       </c>
       <c r="C125" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>963.92954386111501</v>
       </c>
       <c r="D125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>828</v>
       </c>
       <c r="E125" s="3">
@@ -5943,11 +6222,11 @@
         <v>835</v>
       </c>
       <c r="C126" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>950.60360881597433</v>
       </c>
       <c r="D126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>835</v>
       </c>
       <c r="E126" s="3">
@@ -5986,11 +6265,11 @@
         <v>836</v>
       </c>
       <c r="C127" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>676.69812683168027</v>
       </c>
       <c r="D127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>836</v>
       </c>
       <c r="E127" s="3">
@@ -6029,11 +6308,11 @@
         <v>839</v>
       </c>
       <c r="C128" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>983.43431522243338</v>
       </c>
       <c r="D128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>839</v>
       </c>
       <c r="E128" s="3">
@@ -6072,11 +6351,11 @@
         <v>840</v>
       </c>
       <c r="C129" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>768.25489515282618</v>
       </c>
       <c r="D129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>840</v>
       </c>
       <c r="E129" s="3">
@@ -6115,11 +6394,11 @@
         <v>845</v>
       </c>
       <c r="C130" s="4">
-        <f t="shared" ref="C130:C161" si="7">D130*E130</f>
+        <f t="shared" ref="C130:C161" si="8">D130*E130</f>
         <v>804.34030971844402</v>
       </c>
       <c r="D130">
-        <f t="shared" ref="D130:D161" si="8">B130</f>
+        <f t="shared" ref="D130:D161" si="9">B130</f>
         <v>845</v>
       </c>
       <c r="E130" s="3">
@@ -6158,11 +6437,11 @@
         <v>847</v>
       </c>
       <c r="C131" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>767.19747607217914</v>
       </c>
       <c r="D131">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>847</v>
       </c>
       <c r="E131" s="3">
@@ -6201,11 +6480,11 @@
         <v>848</v>
       </c>
       <c r="C132" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>911.71342306523741</v>
       </c>
       <c r="D132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>848</v>
       </c>
       <c r="E132" s="3">
@@ -6244,11 +6523,11 @@
         <v>850</v>
       </c>
       <c r="C133" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>778.7770539028503</v>
       </c>
       <c r="D133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>850</v>
       </c>
       <c r="E133" s="3">
@@ -6287,11 +6566,11 @@
         <v>852</v>
       </c>
       <c r="C134" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1011.6658688265728</v>
       </c>
       <c r="D134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>852</v>
       </c>
       <c r="E134" s="3">
@@ -6330,11 +6609,11 @@
         <v>852</v>
       </c>
       <c r="C135" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>914.86348950739819</v>
       </c>
       <c r="D135">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>852</v>
       </c>
       <c r="E135" s="3">
@@ -6373,11 +6652,11 @@
         <v>853</v>
       </c>
       <c r="C136" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>776.12654818568558</v>
       </c>
       <c r="D136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>853</v>
       </c>
       <c r="E136" s="3">
@@ -6416,11 +6695,11 @@
         <v>853</v>
       </c>
       <c r="C137" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>841.19822782453207</v>
       </c>
       <c r="D137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>853</v>
       </c>
       <c r="E137" s="3">
@@ -6459,11 +6738,11 @@
         <v>877</v>
       </c>
       <c r="C138" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>908.38939633124676</v>
       </c>
       <c r="D138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>877</v>
       </c>
       <c r="E138" s="3">
@@ -6502,11 +6781,11 @@
         <v>881</v>
       </c>
       <c r="C139" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>855.50207451273684</v>
       </c>
       <c r="D139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>881</v>
       </c>
       <c r="E139" s="3">
@@ -6545,11 +6824,11 @@
         <v>886</v>
       </c>
       <c r="C140" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1017.3497317697487</v>
       </c>
       <c r="D140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>886</v>
       </c>
       <c r="E140" s="3">
@@ -6588,11 +6867,11 @@
         <v>900</v>
       </c>
       <c r="C141" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>764.05325196617218</v>
       </c>
       <c r="D141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>900</v>
       </c>
       <c r="E141" s="3">
@@ -6631,11 +6910,11 @@
         <v>702</v>
       </c>
       <c r="C142" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>774.47903600882853</v>
       </c>
       <c r="D142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>702</v>
       </c>
       <c r="E142" s="3">
@@ -6656,7 +6935,7 @@
       <c r="J142">
         <v>0.27100000000000002</v>
       </c>
-      <c r="K142" s="5">
+      <c r="K142">
         <v>100.00700000000001</v>
       </c>
       <c r="L142" s="4">
@@ -6674,11 +6953,11 @@
         <v>705</v>
       </c>
       <c r="C143" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>727.23352078063658</v>
       </c>
       <c r="D143">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>705</v>
       </c>
       <c r="E143" s="3">
@@ -6699,7 +6978,7 @@
       <c r="J143">
         <v>0.52100000000000002</v>
       </c>
-      <c r="K143" s="5">
+      <c r="K143">
         <v>150.99100000000001</v>
       </c>
       <c r="L143" s="4">
@@ -6717,11 +6996,11 @@
         <v>915</v>
       </c>
       <c r="C144" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>770.70090825830027</v>
       </c>
       <c r="D144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>915</v>
       </c>
       <c r="E144" s="3">
@@ -6760,11 +7039,11 @@
         <v>918</v>
       </c>
       <c r="C145" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>778.42911780216275</v>
       </c>
       <c r="D145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>918</v>
       </c>
       <c r="E145" s="3">
@@ -6803,11 +7082,11 @@
         <v>934</v>
       </c>
       <c r="C146" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>781.00959645803027</v>
       </c>
       <c r="D146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>934</v>
       </c>
       <c r="E146" s="3">
@@ -6828,7 +7107,7 @@
       <c r="J146">
         <v>0.18</v>
       </c>
-      <c r="K146" s="5">
+      <c r="K146">
         <v>112.834</v>
       </c>
       <c r="L146" s="4">
@@ -6846,11 +7125,11 @@
         <v>739</v>
       </c>
       <c r="C147" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>821.93444946626937</v>
       </c>
       <c r="D147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>739</v>
       </c>
       <c r="E147" s="3">
@@ -6871,7 +7150,7 @@
       <c r="J147">
         <v>0.80500000000000005</v>
       </c>
-      <c r="K147" s="5">
+      <c r="K147">
         <v>142.94800000000001</v>
       </c>
       <c r="L147" s="4">
@@ -6889,11 +7168,11 @@
         <v>741</v>
       </c>
       <c r="C148" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>859.73600982930407</v>
       </c>
       <c r="D148">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>741</v>
       </c>
       <c r="E148" s="3">
@@ -6914,7 +7193,7 @@
       <c r="J148">
         <v>0.503</v>
       </c>
-      <c r="K148" s="5">
+      <c r="K148">
         <v>156.03299999999999</v>
       </c>
       <c r="L148" s="4">
@@ -6932,11 +7211,11 @@
         <v>946</v>
       </c>
       <c r="C149" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>824.89034524694478</v>
       </c>
       <c r="D149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>946</v>
       </c>
       <c r="E149" s="3">
@@ -6975,11 +7254,11 @@
         <v>947</v>
       </c>
       <c r="C150" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>760.95299171367003</v>
       </c>
       <c r="D150">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>947</v>
       </c>
       <c r="E150" s="3">
@@ -7018,11 +7297,11 @@
         <v>752</v>
       </c>
       <c r="C151" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>889.64434671691583</v>
       </c>
       <c r="D151">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>752</v>
       </c>
       <c r="E151" s="3">
@@ -7043,7 +7322,7 @@
       <c r="J151">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K151" s="5">
+      <c r="K151">
         <v>140.04599999999999</v>
       </c>
       <c r="L151" s="4">
@@ -7061,11 +7340,11 @@
         <v>752</v>
       </c>
       <c r="C152" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>784.11830266730203</v>
       </c>
       <c r="D152">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>752</v>
       </c>
       <c r="E152" s="3">
@@ -7086,7 +7365,7 @@
       <c r="J152">
         <v>7.2400000000000006E-2</v>
       </c>
-      <c r="K152" s="5">
+      <c r="K152">
         <v>144.48099999999999</v>
       </c>
       <c r="L152" s="4">
@@ -7104,11 +7383,11 @@
         <v>757</v>
       </c>
       <c r="C153" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>777.82723633726528</v>
       </c>
       <c r="D153">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>757</v>
       </c>
       <c r="E153" s="3">
@@ -7129,7 +7408,7 @@
       <c r="J153">
         <v>0.69199999999999995</v>
       </c>
-      <c r="K153" s="5">
+      <c r="K153">
         <v>134.99199999999999</v>
       </c>
       <c r="L153" s="4">
@@ -7147,11 +7426,11 @@
         <v>962</v>
       </c>
       <c r="C154" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>975.47763584211941</v>
       </c>
       <c r="D154">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>962</v>
       </c>
       <c r="E154" s="3">
@@ -7190,11 +7469,11 @@
         <v>970</v>
       </c>
       <c r="C155" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>986.40809025809949</v>
       </c>
       <c r="D155">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>970</v>
       </c>
       <c r="E155" s="3">
@@ -7233,11 +7512,11 @@
         <v>974</v>
       </c>
       <c r="C156" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>995.26821967098238</v>
       </c>
       <c r="D156">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>974</v>
       </c>
       <c r="E156" s="3">
@@ -7276,11 +7555,11 @@
         <v>774</v>
       </c>
       <c r="C157" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>691.99736089042779</v>
       </c>
       <c r="D157">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>774</v>
       </c>
       <c r="E157" s="3">
@@ -7301,7 +7580,7 @@
       <c r="J157">
         <v>0.39900000000000002</v>
       </c>
-      <c r="K157" s="5">
+      <c r="K157">
         <v>107.877</v>
       </c>
       <c r="L157" s="4">
@@ -7319,11 +7598,11 @@
         <v>977</v>
       </c>
       <c r="C158" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1161.1614839406413</v>
       </c>
       <c r="D158">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>977</v>
       </c>
       <c r="E158" s="3">
@@ -7344,7 +7623,7 @@
       <c r="J158">
         <v>0.44900000000000001</v>
       </c>
-      <c r="K158" s="5">
+      <c r="K158">
         <v>137.68100000000001</v>
       </c>
       <c r="L158" s="4">
@@ -7362,11 +7641,11 @@
         <v>977</v>
       </c>
       <c r="C159" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>843.62034307532576</v>
       </c>
       <c r="D159">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>977</v>
       </c>
       <c r="E159" s="3">
@@ -7405,11 +7684,11 @@
         <v>780</v>
       </c>
       <c r="C160" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>709.27294546613211</v>
       </c>
       <c r="D160">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>780</v>
       </c>
       <c r="E160" s="3">
@@ -7430,7 +7709,7 @@
       <c r="J160">
         <v>0.25700000000000001</v>
       </c>
-      <c r="K160" s="5">
+      <c r="K160">
         <v>79.792000000000002</v>
       </c>
       <c r="L160" s="4">
@@ -7448,11 +7727,11 @@
         <v>980</v>
       </c>
       <c r="C161" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>989.14863943114563</v>
       </c>
       <c r="D161">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>980</v>
       </c>
       <c r="E161" s="3">
@@ -7491,11 +7770,11 @@
         <v>782</v>
       </c>
       <c r="C162" s="4">
-        <f t="shared" ref="C162:C168" si="9">D162*E162</f>
+        <f t="shared" ref="C162:C168" si="10">D162*E162</f>
         <v>639.51338361095475</v>
       </c>
       <c r="D162">
-        <f t="shared" ref="D162:D193" si="10">B162</f>
+        <f t="shared" ref="D162:D168" si="11">B162</f>
         <v>782</v>
       </c>
       <c r="E162" s="3">
@@ -7516,7 +7795,7 @@
       <c r="J162">
         <v>0.16600000000000001</v>
       </c>
-      <c r="K162" s="5">
+      <c r="K162">
         <v>136.70699999999999</v>
       </c>
       <c r="L162" s="4">
@@ -7534,11 +7813,11 @@
         <v>983</v>
       </c>
       <c r="C163" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>820.64965170868572</v>
       </c>
       <c r="D163">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>983</v>
       </c>
       <c r="E163" s="3">
@@ -7577,11 +7856,11 @@
         <v>986</v>
       </c>
       <c r="C164" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1138.0076919374487</v>
       </c>
       <c r="D164">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>986</v>
       </c>
       <c r="E164" s="3">
@@ -7620,11 +7899,11 @@
         <v>791</v>
       </c>
       <c r="C165" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>635.77007636850419</v>
       </c>
       <c r="D165">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>791</v>
       </c>
       <c r="E165" s="3">
@@ -7645,7 +7924,7 @@
       <c r="J165">
         <v>7.1800000000000003E-2</v>
       </c>
-      <c r="K165" s="5">
+      <c r="K165">
         <v>94.442999999999998</v>
       </c>
       <c r="L165" s="4">
@@ -7663,11 +7942,11 @@
         <v>992</v>
       </c>
       <c r="C166" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>846.18691932122363</v>
       </c>
       <c r="D166">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>992</v>
       </c>
       <c r="E166" s="3">
@@ -7706,11 +7985,11 @@
         <v>993</v>
       </c>
       <c r="C167" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>976.36369568462862</v>
       </c>
       <c r="D167">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>993</v>
       </c>
       <c r="E167" s="3">
@@ -7749,11 +8028,11 @@
         <v>794</v>
       </c>
       <c r="C168" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>775.51445688586773</v>
       </c>
       <c r="D168">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>794</v>
       </c>
       <c r="E168" s="3">
@@ -7774,7 +8053,7 @@
       <c r="J168">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K168" s="5">
+      <c r="K168">
         <v>108.017</v>
       </c>
       <c r="L168" s="4">
@@ -7787,6 +8066,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="D2 D3:D15" calculatedColumn="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Añadir la parte de Hypothesis testing y ya
</commit_message>
<xml_diff>
--- a/Prueba con otros datos/songstats.xlsx
+++ b/Prueba con otros datos/songstats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/Desktop/UC3M/Satistics Final Project/Prueba con otros datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A65C9F0-1B71-9147-B347-D38E56EAC217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B60E7C-C1C9-534D-BCC0-67B223B50669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22400" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{1E92F581-86EA-2D46-99A1-0B3CE0122B65}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1E92F581-86EA-2D46-99A1-0B3CE0122B65}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <dimension ref="A1:O168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>